<commit_message>
update productiedossier + update
</commit_message>
<xml_diff>
--- a/docs/Timesheet_Tine_Vancoillie.xlsx
+++ b/docs/Timesheet_Tine_Vancoillie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="760" yWindow="720" windowWidth="16280" windowHeight="15660" tabRatio="500"/>
+    <workbookView xWindow="760" yWindow="720" windowWidth="28040" windowHeight="15660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -333,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -399,21 +399,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </right>
-      <top style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -553,12 +538,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
@@ -935,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="116" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="143" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,10 +935,10 @@
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1351,7 +1336,7 @@
       <c r="C37" s="10">
         <v>3.75</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="22"/>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
@@ -1374,7 +1359,7 @@
       <c r="C39" s="10">
         <v>4</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
@@ -1648,7 +1633,7 @@
         <v>6</v>
       </c>
       <c r="C64" s="20"/>
-      <c r="E64" s="21"/>
+      <c r="E64" s="24"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1668,7 +1653,7 @@
       <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="22"/>
+      <c r="B68" s="21"/>
       <c r="C68" s="3"/>
     </row>
     <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update + add powerpoint
</commit_message>
<xml_diff>
--- a/docs/Timesheet_Tine_Vancoillie.xlsx
+++ b/docs/Timesheet_Tine_Vancoillie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="760" yWindow="720" windowWidth="28040" windowHeight="15660" tabRatio="500"/>
+    <workbookView xWindow="4660" yWindow="720" windowWidth="23160" windowHeight="15660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Datum</t>
   </si>
@@ -222,6 +222,33 @@
   </si>
   <si>
     <t>Booking status, disabled days home + problems, profile edit</t>
+  </si>
+  <si>
+    <t>info-page, message naar beheer, melding nieuwe request, readme</t>
+  </si>
+  <si>
+    <t>Date home page, book disabled days, profile edit na register, change mail, bugs fixen, change pass</t>
+  </si>
+  <si>
+    <t>add images</t>
+  </si>
+  <si>
+    <t>componentents detail</t>
+  </si>
+  <si>
+    <t>detail + afwerken, request en bookings</t>
+  </si>
+  <si>
+    <t>dossier, disabled days, info page</t>
+  </si>
+  <si>
+    <t>geen review eigen voertuig, contactform</t>
+  </si>
+  <si>
+    <t>afwerken + detail</t>
+  </si>
+  <si>
+    <t>Powerpoint</t>
   </si>
 </sst>
 </file>
@@ -540,10 +567,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
@@ -918,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" zoomScale="143" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,10 +962,10 @@
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1460,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>43087</v>
       </c>
@@ -1471,7 +1498,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>43088</v>
       </c>
@@ -1482,7 +1509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>43091</v>
       </c>
@@ -1493,7 +1520,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>43092</v>
       </c>
@@ -1504,7 +1531,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" s="1" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>43093</v>
       </c>
@@ -1515,7 +1542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>43095</v>
       </c>
@@ -1526,7 +1553,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>43096</v>
       </c>
@@ -1537,7 +1564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>43097</v>
       </c>
@@ -1548,7 +1575,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>43102</v>
       </c>
@@ -1559,7 +1586,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="1" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" s="1" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>43102</v>
       </c>
@@ -1570,7 +1597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>43103</v>
       </c>
@@ -1581,7 +1608,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="1" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" s="1" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>43104</v>
       </c>
@@ -1592,7 +1619,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>43105</v>
       </c>
@@ -1603,7 +1630,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>43105</v>
       </c>
@@ -1614,7 +1641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>43106</v>
       </c>
@@ -1625,89 +1652,143 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="18">
+    <row r="64" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="8">
+        <v>43107</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="8">
+        <v>43108</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="8"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="10"/>
+    </row>
+    <row r="67" spans="1:6" s="1" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="8">
+        <v>43109</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="10">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="1" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="8">
+        <v>43110</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="8">
+        <v>43111</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8">
+        <v>43112</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" s="10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8">
+        <v>43113</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="10">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="8">
+        <v>43114</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72" s="10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="8">
+        <v>43115</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="10">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="18">
         <v>43118</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B74" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="20"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="16" t="s">
+      <c r="C74" s="20"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="17">
-        <f>SUM(C3:C64)</f>
-        <v>225.25</v>
-      </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="21"/>
-      <c r="C68" s="3"/>
-    </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73"/>
-    </row>
-    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-    </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-    </row>
-    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-    </row>
-    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-    </row>
-    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-    </row>
-    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-    </row>
-    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-    </row>
-    <row r="81" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
+      <c r="C75" s="17">
+        <f>SUM(C3:C74)</f>
+        <v>251.5</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B78" s="21"/>
+      <c r="C78" s="3"/>
     </row>
     <row r="83" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
     </row>
     <row r="84" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84"/>
@@ -1774,12 +1855,62 @@
       <c r="B96"/>
       <c r="C96"/>
     </row>
-    <row r="140" ht="46" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97"/>
+      <c r="B97"/>
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98"/>
+      <c r="B98"/>
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99"/>
+      <c r="B99"/>
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100"/>
+      <c r="B100"/>
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103"/>
+      <c r="B103"/>
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104"/>
+      <c r="B104"/>
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106"/>
+      <c r="B106"/>
+      <c r="C106"/>
+    </row>
+    <row r="150" ht="46" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>